<commit_message>
Update Version Numbers to 4.2.0
Updated version number to 4.2.0
</commit_message>
<xml_diff>
--- a/Maps/HOTAS Switch and Button - Quick Reference.xlsx
+++ b/Maps/HOTAS Switch and Button - Quick Reference.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Den\OneDrive\Personal\Thrustmaster\TARGET\Clicker\Development\ED_TargetScript-410b\Maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Den\OneDrive\Personal\Thrustmaster\TARGET\Clicker\Development\ED_TargetScript-420\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -515,9 +515,6 @@
     <t>Launch?</t>
   </si>
   <si>
-    <t>HOTAS - Quick reference - v4.1.0</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -567,6 +564,9 @@
   </si>
   <si>
     <t>tgTriggerDelay</t>
+  </si>
+  <si>
+    <t>HOTAS - Quick reference - v4.2.0</t>
   </si>
 </sst>
 </file>
@@ -1100,24 +1100,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1127,23 +1118,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1431,7 +1431,7 @@
   <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B2" sqref="B2:O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,43 +1456,43 @@
   <sheetData>
     <row r="1" spans="2:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="45"/>
+      <c r="B2" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="54"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="52"/>
-      <c r="G4" s="50" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="48"/>
+      <c r="G4" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="52"/>
-      <c r="L4" s="50" t="s">
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
+      <c r="L4" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="48"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
@@ -1547,21 +1547,21 @@
       <c r="O6" s="15"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="49" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="37"/>
-      <c r="G7" s="46" t="s">
+      <c r="G7" s="43" t="s">
         <v>135</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="32"/>
       <c r="J7" s="21"/>
-      <c r="L7" s="41" t="s">
+      <c r="L7" s="42" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="12" t="s">
@@ -1571,17 +1571,17 @@
       <c r="O7" s="13"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G8" s="47"/>
+        <v>171</v>
+      </c>
+      <c r="G8" s="44"/>
       <c r="H8" s="3" t="s">
         <v>31</v>
       </c>
@@ -1599,17 +1599,17 @@
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="49"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
-      <c r="G9" s="47"/>
+      <c r="G9" s="44"/>
       <c r="H9" s="3"/>
       <c r="I9" s="33"/>
       <c r="J9" s="23"/>
-      <c r="L9" s="42"/>
+      <c r="L9" s="40"/>
       <c r="M9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1617,17 +1617,17 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="49"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G10" s="47" t="s">
+        <v>170</v>
+      </c>
+      <c r="G10" s="44" t="s">
         <v>136</v>
       </c>
       <c r="H10" s="3"/>
@@ -1643,15 +1643,15 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="49"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="G11" s="47"/>
+      <c r="G11" s="44"/>
       <c r="H11" s="28" t="s">
         <v>31</v>
       </c>
@@ -1669,21 +1669,21 @@
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="54"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" s="47"/>
+        <v>172</v>
+      </c>
+      <c r="G12" s="44"/>
       <c r="H12" s="3"/>
       <c r="I12" s="33"/>
       <c r="J12" s="23"/>
-      <c r="L12" s="42"/>
+      <c r="L12" s="40"/>
       <c r="M12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1691,7 +1691,7 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="50" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
-      <c r="G13" s="47" t="s">
+      <c r="G13" s="44" t="s">
         <v>137</v>
       </c>
       <c r="H13" s="3"/>
@@ -1715,13 +1715,13 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="49"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="24"/>
-      <c r="G14" s="47"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="3" t="s">
         <v>31</v>
       </c>
@@ -1739,17 +1739,17 @@
       <c r="O14" s="4"/>
     </row>
     <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="40"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="6"/>
-      <c r="G15" s="48"/>
+      <c r="G15" s="45"/>
       <c r="H15" s="27"/>
       <c r="I15" s="33"/>
       <c r="J15" s="23"/>
-      <c r="L15" s="40"/>
+      <c r="L15" s="41"/>
       <c r="M15" s="5" t="s">
         <v>32</v>
       </c>
@@ -1767,7 +1767,7 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -1777,7 +1777,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="G17" s="46" t="s">
+      <c r="G17" s="43" t="s">
         <v>58</v>
       </c>
       <c r="H17" s="12" t="s">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="13"/>
-      <c r="L17" s="41" t="s">
+      <c r="L17" s="42" t="s">
         <v>84</v>
       </c>
       <c r="M17" s="12" t="s">
@@ -1803,7 +1803,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="G18" s="47"/>
+      <c r="G18" s="44"/>
       <c r="H18" s="3" t="s">
         <v>31</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="O18" s="4"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
@@ -1829,7 +1829,7 @@
       <c r="E19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="48"/>
+      <c r="G19" s="45"/>
       <c r="H19" s="5" t="s">
         <v>32</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>60</v>
       </c>
       <c r="J19" s="6"/>
-      <c r="L19" s="42"/>
+      <c r="L19" s="40"/>
       <c r="M19" s="3" t="s">
         <v>32</v>
       </c>
@@ -1863,15 +1863,15 @@
       <c r="O20" s="4"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="43" t="s">
         <v>132</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="37"/>
-      <c r="G21" s="46" t="s">
+      <c r="G21" s="43" t="s">
         <v>61</v>
       </c>
       <c r="H21" s="29" t="s">
@@ -1889,17 +1889,17 @@
       <c r="O21" s="4"/>
     </row>
     <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="47"/>
+      <c r="B22" s="44"/>
       <c r="C22" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>134</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="G22" s="47"/>
+        <v>171</v>
+      </c>
+      <c r="G22" s="44"/>
       <c r="H22" s="3" t="s">
         <v>31</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>62</v>
       </c>
       <c r="J22" s="4"/>
-      <c r="L22" s="40"/>
+      <c r="L22" s="41"/>
       <c r="M22" s="5" t="s">
         <v>32</v>
       </c>
@@ -1915,13 +1915,13 @@
       <c r="O22" s="6"/>
     </row>
     <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47"/>
+      <c r="B23" s="44"/>
       <c r="C23" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
-      <c r="G23" s="48"/>
+      <c r="G23" s="45"/>
       <c r="H23" s="5" t="s">
         <v>32</v>
       </c>
@@ -1931,21 +1931,21 @@
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="47"/>
+      <c r="B24" s="44"/>
       <c r="C24" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>134</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="L24" s="41" t="s">
+      <c r="L24" s="42" t="s">
         <v>86</v>
       </c>
       <c r="M24" s="12" t="s">
@@ -1955,15 +1955,15 @@
       <c r="O24" s="13"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="47"/>
+      <c r="B25" s="44"/>
       <c r="C25" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="G25" s="41" t="s">
+      <c r="G25" s="42" t="s">
         <v>63</v>
       </c>
       <c r="H25" s="12" t="s">
@@ -1981,15 +1981,15 @@
       <c r="O25" s="4"/>
     </row>
     <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="48"/>
+      <c r="B26" s="45"/>
       <c r="C26" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G26" s="39"/>
       <c r="H26" s="3" t="s">
@@ -1999,7 +1999,7 @@
         <v>130</v>
       </c>
       <c r="J26" s="4"/>
-      <c r="L26" s="42"/>
+      <c r="L26" s="40"/>
       <c r="M26" s="3" t="s">
         <v>32</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="G27" s="42"/>
+      <c r="G27" s="40"/>
       <c r="H27" s="3" t="s">
         <v>32</v>
       </c>
@@ -2027,7 +2027,7 @@
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="42" t="s">
         <v>133</v>
       </c>
       <c r="C28" s="18" t="s">
@@ -2069,7 +2069,7 @@
         <v>131</v>
       </c>
       <c r="J29" s="4"/>
-      <c r="L29" s="40"/>
+      <c r="L29" s="41"/>
       <c r="M29" s="5" t="s">
         <v>32</v>
       </c>
@@ -2077,13 +2077,13 @@
       <c r="O29" s="6"/>
     </row>
     <row r="30" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="40"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="23"/>
-      <c r="G30" s="42"/>
+      <c r="G30" s="40"/>
       <c r="H30" s="3" t="s">
         <v>32</v>
       </c>
@@ -2103,7 +2103,7 @@
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="4"/>
-      <c r="L31" s="41" t="s">
+      <c r="L31" s="42" t="s">
         <v>88</v>
       </c>
       <c r="M31" s="12" t="s">
@@ -2113,7 +2113,7 @@
       <c r="O31" s="13"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="41" t="s">
+      <c r="B32" s="42" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -2147,13 +2147,13 @@
         <v>5</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="G33" s="42"/>
+      <c r="G33" s="40"/>
       <c r="H33" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="4"/>
-      <c r="L33" s="40"/>
+      <c r="L33" s="41"/>
       <c r="M33" s="5" t="s">
         <v>32</v>
       </c>
@@ -2161,7 +2161,7 @@
       <c r="O33" s="6"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="40"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="5" t="s">
         <v>32</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>110</v>
       </c>
       <c r="J35" s="4"/>
-      <c r="L35" s="41" t="s">
+      <c r="L35" s="42" t="s">
         <v>89</v>
       </c>
       <c r="M35" s="12" t="s">
@@ -2199,7 +2199,7 @@
       <c r="O35" s="13"/>
     </row>
     <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="42" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -2209,7 +2209,7 @@
         <v>6</v>
       </c>
       <c r="E36" s="13"/>
-      <c r="G36" s="40"/>
+      <c r="G36" s="41"/>
       <c r="H36" s="5" t="s">
         <v>32</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="L37" s="40"/>
+      <c r="L37" s="41"/>
       <c r="M37" s="5" t="s">
         <v>32</v>
       </c>
@@ -2241,7 +2241,7 @@
       <c r="O37" s="6"/>
     </row>
     <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="42"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="3" t="s">
         <v>32</v>
       </c>
@@ -2249,14 +2249,14 @@
         <v>8</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="G38" s="41" t="s">
+      <c r="G38" s="42" t="s">
         <v>67</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J38" s="13"/>
     </row>
@@ -2271,11 +2271,11 @@
       <c r="E39" s="4"/>
       <c r="G39" s="39"/>
       <c r="H39" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="4"/>
-      <c r="L39" s="41" t="s">
+      <c r="L39" s="42" t="s">
         <v>90</v>
       </c>
       <c r="M39" s="12" t="s">
@@ -2293,7 +2293,7 @@
         <v>9</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="G40" s="42"/>
+      <c r="G40" s="40"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
       <c r="J40" s="22"/>
@@ -2307,7 +2307,7 @@
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="42"/>
+      <c r="B41" s="40"/>
       <c r="C41" s="3" t="s">
         <v>32</v>
       </c>
@@ -2317,13 +2317,13 @@
         <v>68</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J41" s="4"/>
-      <c r="L41" s="42"/>
+      <c r="L41" s="40"/>
       <c r="M41" s="3" t="s">
         <v>32</v>
       </c>
@@ -2341,7 +2341,7 @@
       <c r="E42" s="4"/>
       <c r="G42" s="39"/>
       <c r="H42" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="4"/>
@@ -2363,7 +2363,7 @@
         <v>10</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="G43" s="42"/>
+      <c r="G43" s="40"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
       <c r="J43" s="22"/>
@@ -2377,7 +2377,7 @@
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="42"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="3" t="s">
         <v>32</v>
       </c>
@@ -2387,13 +2387,13 @@
         <v>69</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J44" s="4"/>
-      <c r="L44" s="42"/>
+      <c r="L44" s="40"/>
       <c r="M44" s="3" t="s">
         <v>32</v>
       </c>
@@ -2415,7 +2415,7 @@
       <c r="E45" s="4"/>
       <c r="G45" s="39"/>
       <c r="H45" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="4"/>
@@ -2437,7 +2437,7 @@
         <v>11</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="G46" s="42"/>
+      <c r="G46" s="40"/>
       <c r="H46" s="34"/>
       <c r="I46" s="34"/>
       <c r="J46" s="22"/>
@@ -2451,7 +2451,7 @@
       <c r="O46" s="4"/>
     </row>
     <row r="47" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="40"/>
+      <c r="B47" s="41"/>
       <c r="C47" s="5" t="s">
         <v>32</v>
       </c>
@@ -2463,13 +2463,13 @@
         <v>70</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J47" s="4"/>
-      <c r="L47" s="40"/>
+      <c r="L47" s="41"/>
       <c r="M47" s="5" t="s">
         <v>32</v>
       </c>
@@ -2485,13 +2485,13 @@
       <c r="E48" s="15"/>
       <c r="G48" s="39"/>
       <c r="H48" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="41" t="s">
+      <c r="B49" s="42" t="s">
         <v>39</v>
       </c>
       <c r="C49" s="12" t="s">
@@ -2501,11 +2501,11 @@
         <v>12</v>
       </c>
       <c r="E49" s="13"/>
-      <c r="G49" s="42"/>
+      <c r="G49" s="40"/>
       <c r="H49" s="34"/>
       <c r="I49" s="34"/>
       <c r="J49" s="22"/>
-      <c r="L49" s="41" t="s">
+      <c r="L49" s="42" t="s">
         <v>93</v>
       </c>
       <c r="M49" s="12" t="s">
@@ -2527,10 +2527,10 @@
         <v>71</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J50" s="4"/>
       <c r="L50" s="39"/>
@@ -2543,7 +2543,7 @@
       <c r="O50" s="4"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="42"/>
+      <c r="B51" s="40"/>
       <c r="C51" s="3" t="s">
         <v>32</v>
       </c>
@@ -2551,13 +2551,13 @@
       <c r="E51" s="4"/>
       <c r="G51" s="39"/>
       <c r="H51" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="J51" s="4"/>
-      <c r="L51" s="42"/>
+      <c r="L51" s="40"/>
       <c r="M51" s="3" t="s">
         <v>32</v>
       </c>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
-      <c r="G52" s="40"/>
+      <c r="G52" s="41"/>
       <c r="H52" s="35"/>
       <c r="I52" s="35"/>
       <c r="J52" s="23"/>
@@ -2605,7 +2605,7 @@
       <c r="O53" s="4"/>
     </row>
     <row r="54" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="42"/>
+      <c r="B54" s="40"/>
       <c r="C54" s="3" t="s">
         <v>32</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>15</v>
       </c>
       <c r="E54" s="4"/>
-      <c r="G54" s="41" t="s">
+      <c r="G54" s="42" t="s">
         <v>72</v>
       </c>
       <c r="H54" s="12" t="s">
@@ -2623,7 +2623,7 @@
         <v>152</v>
       </c>
       <c r="J54" s="13"/>
-      <c r="L54" s="40"/>
+      <c r="L54" s="41"/>
       <c r="M54" s="5" t="s">
         <v>32</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>16</v>
       </c>
       <c r="E56" s="4"/>
-      <c r="G56" s="42"/>
+      <c r="G56" s="40"/>
       <c r="H56" s="3" t="s">
         <v>32</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>154</v>
       </c>
       <c r="J56" s="4"/>
-      <c r="L56" s="41" t="s">
+      <c r="L56" s="42" t="s">
         <v>95</v>
       </c>
       <c r="M56" s="12" t="s">
@@ -2675,7 +2675,7 @@
       <c r="O56" s="13"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="42"/>
+      <c r="B57" s="40"/>
       <c r="C57" s="3" t="s">
         <v>32</v>
       </c>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="I58" s="7"/>
       <c r="J58" s="8"/>
-      <c r="L58" s="42"/>
+      <c r="L58" s="40"/>
       <c r="M58" s="3" t="s">
         <v>32</v>
       </c>
@@ -2751,7 +2751,7 @@
       <c r="O59" s="4"/>
     </row>
     <row r="60" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="40"/>
+      <c r="B60" s="41"/>
       <c r="C60" s="5" t="s">
         <v>32</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>19</v>
       </c>
       <c r="E60" s="6"/>
-      <c r="G60" s="40"/>
+      <c r="G60" s="41"/>
       <c r="H60" s="5" t="s">
         <v>32</v>
       </c>
@@ -2777,7 +2777,7 @@
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
-      <c r="L61" s="42"/>
+      <c r="L61" s="40"/>
       <c r="M61" s="3" t="s">
         <v>32</v>
       </c>
@@ -2785,7 +2785,7 @@
       <c r="O61" s="4"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="41" t="s">
+      <c r="B62" s="42" t="s">
         <v>43</v>
       </c>
       <c r="C62" s="12" t="s">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
-      <c r="G62" s="41" t="s">
+      <c r="G62" s="42" t="s">
         <v>76</v>
       </c>
       <c r="H62" s="12" t="s">
@@ -2837,19 +2837,19 @@
       <c r="O63" s="4"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="42"/>
+      <c r="B64" s="40"/>
       <c r="C64" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
-      <c r="G64" s="42"/>
+      <c r="G64" s="40"/>
       <c r="H64" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="4"/>
-      <c r="L64" s="42"/>
+      <c r="L64" s="40"/>
       <c r="M64" s="3" t="s">
         <v>32</v>
       </c>
@@ -2899,19 +2899,19 @@
       <c r="J66" s="4"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="42"/>
+      <c r="B67" s="40"/>
       <c r="C67" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
-      <c r="G67" s="42"/>
+      <c r="G67" s="40"/>
       <c r="H67" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I67" s="3"/>
       <c r="J67" s="4"/>
-      <c r="L67" s="41" t="s">
+      <c r="L67" s="42" t="s">
         <v>99</v>
       </c>
       <c r="M67" s="12" t="s">
@@ -2965,7 +2965,7 @@
         <v>112</v>
       </c>
       <c r="J69" s="4"/>
-      <c r="L69" s="42"/>
+      <c r="L69" s="40"/>
       <c r="M69" s="3" t="s">
         <v>32</v>
       </c>
@@ -2975,13 +2975,13 @@
       <c r="O69" s="4"/>
     </row>
     <row r="70" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="42"/>
+      <c r="B70" s="40"/>
       <c r="C70" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
-      <c r="G70" s="40"/>
+      <c r="G70" s="41"/>
       <c r="H70" s="5" t="s">
         <v>32</v>
       </c>
@@ -3021,7 +3021,7 @@
         <v>20</v>
       </c>
       <c r="E72" s="4"/>
-      <c r="G72" s="41" t="s">
+      <c r="G72" s="42" t="s">
         <v>79</v>
       </c>
       <c r="H72" s="12" t="s">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="I72" s="12"/>
       <c r="J72" s="13"/>
-      <c r="L72" s="42"/>
+      <c r="L72" s="40"/>
       <c r="M72" s="3" t="s">
         <v>32</v>
       </c>
@@ -3037,7 +3037,7 @@
       <c r="O72" s="4"/>
     </row>
     <row r="73" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="40"/>
+      <c r="B73" s="41"/>
       <c r="C73" s="5" t="s">
         <v>32</v>
       </c>
@@ -3065,7 +3065,7 @@
       <c r="C74" s="15"/>
       <c r="D74" s="15"/>
       <c r="E74" s="15"/>
-      <c r="G74" s="42"/>
+      <c r="G74" s="40"/>
       <c r="H74" s="3" t="s">
         <v>32</v>
       </c>
@@ -3079,7 +3079,7 @@
       <c r="O74" s="4"/>
     </row>
     <row r="75" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="41" t="s">
+      <c r="B75" s="42" t="s">
         <v>47</v>
       </c>
       <c r="C75" s="12" t="s">
@@ -3097,7 +3097,7 @@
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="4"/>
-      <c r="L75" s="40"/>
+      <c r="L75" s="41"/>
       <c r="M75" s="5" t="s">
         <v>32</v>
       </c>
@@ -3123,7 +3123,7 @@
       <c r="J76" s="4"/>
     </row>
     <row r="77" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="42"/>
+      <c r="B77" s="40"/>
       <c r="C77" s="3" t="s">
         <v>32</v>
       </c>
@@ -3131,13 +3131,13 @@
         <v>22</v>
       </c>
       <c r="E77" s="31"/>
-      <c r="G77" s="40"/>
+      <c r="G77" s="41"/>
       <c r="H77" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="6"/>
-      <c r="L77" s="41" t="s">
+      <c r="L77" s="42" t="s">
         <v>102</v>
       </c>
       <c r="M77" s="12" t="s">
@@ -3179,7 +3179,7 @@
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="2"/>
-      <c r="L79" s="42"/>
+      <c r="L79" s="40"/>
       <c r="M79" s="3" t="s">
         <v>32</v>
       </c>
@@ -3190,7 +3190,7 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
-      <c r="B80" s="42"/>
+      <c r="B80" s="40"/>
       <c r="C80" s="3" t="s">
         <v>32</v>
       </c>
@@ -3233,7 +3233,7 @@
         <v>144</v>
       </c>
       <c r="E82" s="4"/>
-      <c r="L82" s="40"/>
+      <c r="L82" s="41"/>
       <c r="M82" s="5" t="s">
         <v>32</v>
       </c>
@@ -3241,7 +3241,7 @@
       <c r="O82" s="6"/>
     </row>
     <row r="83" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="42"/>
+      <c r="B83" s="40"/>
       <c r="C83" s="3" t="s">
         <v>32</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>0</v>
       </c>
       <c r="E84" s="4"/>
-      <c r="L84" s="41" t="s">
+      <c r="L84" s="42" t="s">
         <v>104</v>
       </c>
       <c r="M84" s="12" t="s">
@@ -3291,7 +3291,7 @@
       <c r="O85" s="4"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="42"/>
+      <c r="B86" s="40"/>
       <c r="C86" s="3" t="s">
         <v>32</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>0</v>
       </c>
       <c r="E86" s="4"/>
-      <c r="L86" s="42"/>
+      <c r="L86" s="40"/>
       <c r="M86" s="3" t="s">
         <v>32</v>
       </c>
@@ -3341,7 +3341,7 @@
       <c r="O88" s="4"/>
     </row>
     <row r="89" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="42"/>
+      <c r="B89" s="40"/>
       <c r="C89" s="3" t="s">
         <v>32</v>
       </c>
@@ -3349,7 +3349,7 @@
         <v>27</v>
       </c>
       <c r="E89" s="31"/>
-      <c r="L89" s="40"/>
+      <c r="L89" s="41"/>
       <c r="M89" s="5" t="s">
         <v>32</v>
       </c>
@@ -3377,7 +3377,7 @@
         <v>150</v>
       </c>
       <c r="E91" s="4"/>
-      <c r="L91" s="41" t="s">
+      <c r="L91" s="42" t="s">
         <v>105</v>
       </c>
       <c r="M91" s="12" t="s">
@@ -3387,7 +3387,7 @@
       <c r="O91" s="13"/>
     </row>
     <row r="92" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="40"/>
+      <c r="B92" s="41"/>
       <c r="C92" s="5" t="s">
         <v>32</v>
       </c>
@@ -3405,7 +3405,7 @@
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L93" s="42"/>
+      <c r="L93" s="40"/>
       <c r="M93" s="3" t="s">
         <v>32</v>
       </c>
@@ -3433,7 +3433,7 @@
       </c>
     </row>
     <row r="96" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L96" s="40"/>
+      <c r="L96" s="41"/>
       <c r="M96" s="5" t="s">
         <v>32</v>
       </c>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="97" spans="12:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L98" s="41" t="s">
+      <c r="L98" s="42" t="s">
         <v>107</v>
       </c>
       <c r="M98" s="12" t="s">
@@ -3460,7 +3460,7 @@
       <c r="O99" s="4"/>
     </row>
     <row r="100" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L100" s="42"/>
+      <c r="L100" s="40"/>
       <c r="M100" s="3" t="s">
         <v>32</v>
       </c>
@@ -3486,7 +3486,7 @@
       <c r="O102" s="4"/>
     </row>
     <row r="103" spans="12:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L103" s="40"/>
+      <c r="L103" s="41"/>
       <c r="M103" s="5" t="s">
         <v>32</v>
       </c>
@@ -3495,11 +3495,60 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="L70:L72"/>
-    <mergeCell ref="L73:L75"/>
-    <mergeCell ref="L77:L79"/>
-    <mergeCell ref="L80:L82"/>
+    <mergeCell ref="L87:L89"/>
+    <mergeCell ref="L91:L93"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="L98:L100"/>
+    <mergeCell ref="L101:L103"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="G58:G60"/>
+    <mergeCell ref="G62:G64"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="G38:G40"/>
+    <mergeCell ref="G41:G43"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="B71:B73"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="L45:L47"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="L39:L41"/>
+    <mergeCell ref="L42:L44"/>
     <mergeCell ref="B87:B89"/>
     <mergeCell ref="L84:L86"/>
     <mergeCell ref="L67:L69"/>
@@ -3516,62 +3565,13 @@
     <mergeCell ref="L62:L64"/>
     <mergeCell ref="G65:G67"/>
     <mergeCell ref="G68:G70"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="L70:L72"/>
+    <mergeCell ref="L73:L75"/>
+    <mergeCell ref="L77:L79"/>
+    <mergeCell ref="L80:L82"/>
     <mergeCell ref="G72:G74"/>
     <mergeCell ref="G75:G77"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="L10:L12"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="L39:L41"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="L45:L47"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G47:G49"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="G54:G56"/>
-    <mergeCell ref="G58:G60"/>
-    <mergeCell ref="G62:G64"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="G38:G40"/>
-    <mergeCell ref="G41:G43"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="L87:L89"/>
-    <mergeCell ref="L91:L93"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="L98:L100"/>
-    <mergeCell ref="L101:L103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update HOTAS Switch and Button - Quick Reference.xlsx
Updated for LDGH and FLAPS switch usage
</commit_message>
<xml_diff>
--- a/Maps/HOTAS Switch and Button - Quick Reference.xlsx
+++ b/Maps/HOTAS Switch and Button - Quick Reference.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="182">
   <si>
     <t>TG1</t>
   </si>
@@ -377,18 +377,9 @@
     <t>tgCargoScoop()</t>
   </si>
   <si>
-    <t>mTextCLEARChatBox</t>
-  </si>
-  <si>
     <t>fnRequestDock()</t>
   </si>
   <si>
-    <t>SetLED OFF</t>
-  </si>
-  <si>
-    <t>SetLED ON</t>
-  </si>
-  <si>
     <t>fnDeploySRV()</t>
   </si>
   <si>
@@ -500,15 +491,6 @@
     <t>fnSetJoystickCurves(2)</t>
   </si>
   <si>
-    <t>fnSliderCurve(0)</t>
-  </si>
-  <si>
-    <t>fnSliderCurve(1)</t>
-  </si>
-  <si>
-    <t>fnSliderCurve(2)</t>
-  </si>
-  <si>
     <t>Enter Hanger?</t>
   </si>
   <si>
@@ -567,6 +549,27 @@
   </si>
   <si>
     <t>HOTAS - Quick reference - v4.2.0</t>
+  </si>
+  <si>
+    <t>mClearAllChatBox</t>
+  </si>
+  <si>
+    <t>mClearChatBox</t>
+  </si>
+  <si>
+    <t>fnVoiceVolume(INCREASE)</t>
+  </si>
+  <si>
+    <t>Galaxy Map</t>
+  </si>
+  <si>
+    <t>fnVoiceVolume(DECREASE)</t>
+  </si>
+  <si>
+    <t>SystemMap</t>
+  </si>
+  <si>
+    <t>SetLED OFF/ON</t>
   </si>
 </sst>
 </file>
@@ -610,7 +613,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -977,11 +980,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1094,20 +1110,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1118,6 +1149,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1130,19 +1164,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1430,8 +1455,8 @@
   </sheetPr>
   <dimension ref="A1:O103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:O2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,43 +1481,43 @@
   <sheetData>
     <row r="1" spans="2:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="52" t="s">
-        <v>180</v>
-      </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="54"/>
+      <c r="B2" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="47"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="48"/>
-      <c r="G4" s="46" t="s">
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54"/>
+      <c r="G4" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="48"/>
-      <c r="L4" s="46" t="s">
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="54"/>
+      <c r="L4" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="48"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="54"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9" t="s">
@@ -1547,21 +1572,21 @@
       <c r="O6" s="15"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="55" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="37"/>
-      <c r="G7" s="43" t="s">
-        <v>135</v>
+      <c r="G7" s="48" t="s">
+        <v>132</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="32"/>
       <c r="J7" s="21"/>
-      <c r="L7" s="42" t="s">
+      <c r="L7" s="43" t="s">
         <v>81</v>
       </c>
       <c r="M7" s="12" t="s">
@@ -1571,45 +1596,45 @@
       <c r="O7" s="13"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="50"/>
+      <c r="B8" s="51"/>
       <c r="C8" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G8" s="44"/>
+        <v>165</v>
+      </c>
+      <c r="G8" s="49"/>
       <c r="H8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J8" s="22"/>
-      <c r="L8" s="39"/>
+      <c r="L8" s="41"/>
       <c r="M8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="O8" s="4"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="50"/>
+      <c r="B9" s="51"/>
       <c r="C9" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="4"/>
-      <c r="G9" s="44"/>
+      <c r="G9" s="49"/>
       <c r="H9" s="3"/>
       <c r="I9" s="33"/>
       <c r="J9" s="23"/>
-      <c r="L9" s="40"/>
+      <c r="L9" s="44"/>
       <c r="M9" s="3" t="s">
         <v>32</v>
       </c>
@@ -1617,23 +1642,23 @@
       <c r="O9" s="4"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="50"/>
+      <c r="B10" s="51"/>
       <c r="C10" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G10" s="44" t="s">
-        <v>136</v>
+        <v>164</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>133</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="32"/>
       <c r="J10" s="21"/>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="40" t="s">
         <v>82</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1643,47 +1668,47 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="50"/>
+      <c r="B11" s="51"/>
       <c r="C11" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="G11" s="44"/>
+      <c r="G11" s="49"/>
       <c r="H11" s="28" t="s">
         <v>31</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J11" s="22"/>
-      <c r="L11" s="39"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="O11" s="4"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="51"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G12" s="44"/>
+        <v>166</v>
+      </c>
+      <c r="G12" s="49"/>
       <c r="H12" s="3"/>
       <c r="I12" s="33"/>
       <c r="J12" s="23"/>
-      <c r="L12" s="40"/>
+      <c r="L12" s="44"/>
       <c r="M12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1691,7 +1716,7 @@
       <c r="O12" s="4"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="51" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
@@ -1699,13 +1724,13 @@
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="8"/>
-      <c r="G13" s="44" t="s">
-        <v>137</v>
+      <c r="G13" s="49" t="s">
+        <v>134</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="32"/>
       <c r="J13" s="21"/>
-      <c r="L13" s="38" t="s">
+      <c r="L13" s="40" t="s">
         <v>83</v>
       </c>
       <c r="M13" s="3" t="s">
@@ -1715,41 +1740,41 @@
       <c r="O13" s="4"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="50"/>
+      <c r="B14" s="51"/>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="24"/>
-      <c r="G14" s="44"/>
+      <c r="G14" s="49"/>
       <c r="H14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J14" s="22"/>
-      <c r="L14" s="39"/>
+      <c r="L14" s="41"/>
       <c r="M14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O14" s="4"/>
     </row>
     <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="41"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="6"/>
-      <c r="G15" s="45"/>
+      <c r="G15" s="50"/>
       <c r="H15" s="27"/>
       <c r="I15" s="33"/>
       <c r="J15" s="23"/>
-      <c r="L15" s="41"/>
+      <c r="L15" s="42"/>
       <c r="M15" s="5" t="s">
         <v>32</v>
       </c>
@@ -1767,7 +1792,7 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="43" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -1777,7 +1802,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="13"/>
-      <c r="G17" s="43" t="s">
+      <c r="G17" s="48" t="s">
         <v>58</v>
       </c>
       <c r="H17" s="12" t="s">
@@ -1785,7 +1810,7 @@
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="13"/>
-      <c r="L17" s="42" t="s">
+      <c r="L17" s="43" t="s">
         <v>84</v>
       </c>
       <c r="M17" s="12" t="s">
@@ -1795,7 +1820,7 @@
       <c r="O17" s="13"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
@@ -1803,7 +1828,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="G18" s="44"/>
+      <c r="G18" s="49"/>
       <c r="H18" s="3" t="s">
         <v>31</v>
       </c>
@@ -1811,7 +1836,7 @@
         <v>59</v>
       </c>
       <c r="J18" s="4"/>
-      <c r="L18" s="39"/>
+      <c r="L18" s="41"/>
       <c r="M18" s="3" t="s">
         <v>31</v>
       </c>
@@ -1821,7 +1846,7 @@
       <c r="O18" s="4"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="41"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="5" t="s">
         <v>32</v>
       </c>
@@ -1829,7 +1854,7 @@
       <c r="E19" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="45"/>
+      <c r="G19" s="50"/>
       <c r="H19" s="5" t="s">
         <v>32</v>
       </c>
@@ -1837,7 +1862,7 @@
         <v>60</v>
       </c>
       <c r="J19" s="6"/>
-      <c r="L19" s="40"/>
+      <c r="L19" s="44"/>
       <c r="M19" s="3" t="s">
         <v>32</v>
       </c>
@@ -1853,7 +1878,7 @@
       <c r="H20" s="15"/>
       <c r="I20" s="15"/>
       <c r="J20" s="15"/>
-      <c r="L20" s="38" t="s">
+      <c r="L20" s="40" t="s">
         <v>85</v>
       </c>
       <c r="M20" s="3" t="s">
@@ -1863,15 +1888,15 @@
       <c r="O20" s="4"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="s">
-        <v>132</v>
+      <c r="B21" s="48" t="s">
+        <v>129</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D21" s="36"/>
       <c r="E21" s="37"/>
-      <c r="G21" s="43" t="s">
+      <c r="G21" s="48" t="s">
         <v>61</v>
       </c>
       <c r="H21" s="29" t="s">
@@ -1879,7 +1904,7 @@
       </c>
       <c r="I21" s="29"/>
       <c r="J21" s="30"/>
-      <c r="L21" s="39"/>
+      <c r="L21" s="41"/>
       <c r="M21" s="3" t="s">
         <v>31</v>
       </c>
@@ -1889,17 +1914,17 @@
       <c r="O21" s="4"/>
     </row>
     <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="44"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G22" s="44"/>
+        <v>165</v>
+      </c>
+      <c r="G22" s="49"/>
       <c r="H22" s="3" t="s">
         <v>31</v>
       </c>
@@ -1907,7 +1932,7 @@
         <v>62</v>
       </c>
       <c r="J22" s="4"/>
-      <c r="L22" s="41"/>
+      <c r="L22" s="42"/>
       <c r="M22" s="5" t="s">
         <v>32</v>
       </c>
@@ -1915,37 +1940,37 @@
       <c r="O22" s="6"/>
     </row>
     <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="44"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="4"/>
-      <c r="G23" s="45"/>
+      <c r="G23" s="50"/>
       <c r="H23" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J23" s="6"/>
     </row>
     <row r="24" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="44"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15"/>
-      <c r="L24" s="42" t="s">
+      <c r="L24" s="43" t="s">
         <v>86</v>
       </c>
       <c r="M24" s="12" t="s">
@@ -1955,15 +1980,15 @@
       <c r="O24" s="13"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="44"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E25" s="4"/>
-      <c r="G25" s="42" t="s">
+      <c r="G25" s="43" t="s">
         <v>63</v>
       </c>
       <c r="H25" s="12" t="s">
@@ -1971,7 +1996,7 @@
       </c>
       <c r="I25" s="12"/>
       <c r="J25" s="13"/>
-      <c r="L25" s="39"/>
+      <c r="L25" s="41"/>
       <c r="M25" s="3" t="s">
         <v>31</v>
       </c>
@@ -1981,25 +2006,25 @@
       <c r="O25" s="4"/>
     </row>
     <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="45"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="5" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G26" s="39"/>
+        <v>166</v>
+      </c>
+      <c r="G26" s="41"/>
       <c r="H26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J26" s="4"/>
-      <c r="L26" s="40"/>
+      <c r="L26" s="44"/>
       <c r="M26" s="3" t="s">
         <v>32</v>
       </c>
@@ -2011,13 +2036,13 @@
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="G27" s="40"/>
+      <c r="G27" s="44"/>
       <c r="H27" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I27" s="3"/>
       <c r="J27" s="4"/>
-      <c r="L27" s="38" t="s">
+      <c r="L27" s="40" t="s">
         <v>87</v>
       </c>
       <c r="M27" s="3" t="s">
@@ -2027,15 +2052,15 @@
       <c r="O27" s="4"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="42" t="s">
-        <v>133</v>
+      <c r="B28" s="43" t="s">
+        <v>130</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="32"/>
       <c r="E28" s="21"/>
-      <c r="G28" s="38" t="s">
+      <c r="G28" s="40" t="s">
         <v>64</v>
       </c>
       <c r="H28" s="3" t="s">
@@ -2043,7 +2068,7 @@
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="4"/>
-      <c r="L28" s="39"/>
+      <c r="L28" s="41"/>
       <c r="M28" s="3" t="s">
         <v>31</v>
       </c>
@@ -2053,23 +2078,23 @@
       <c r="O28" s="4"/>
     </row>
     <row r="29" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="39"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E29" s="22"/>
-      <c r="G29" s="39"/>
+      <c r="G29" s="41"/>
       <c r="H29" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J29" s="4"/>
-      <c r="L29" s="41"/>
+      <c r="L29" s="42"/>
       <c r="M29" s="5" t="s">
         <v>32</v>
       </c>
@@ -2077,13 +2102,13 @@
       <c r="O29" s="6"/>
     </row>
     <row r="30" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="41"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="33"/>
       <c r="E30" s="23"/>
-      <c r="G30" s="40"/>
+      <c r="G30" s="44"/>
       <c r="H30" s="3" t="s">
         <v>32</v>
       </c>
@@ -2095,7 +2120,7 @@
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
-      <c r="G31" s="38" t="s">
+      <c r="G31" s="40" t="s">
         <v>65</v>
       </c>
       <c r="H31" s="3" t="s">
@@ -2103,17 +2128,19 @@
       </c>
       <c r="I31" s="3"/>
       <c r="J31" s="4"/>
-      <c r="L31" s="42" t="s">
+      <c r="L31" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="M31" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="N31" s="12"/>
-      <c r="O31" s="13"/>
+      <c r="M31" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="N31" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="O31" s="39"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="43" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -2121,7 +2148,7 @@
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="13"/>
-      <c r="G32" s="39"/>
+      <c r="G32" s="41"/>
       <c r="H32" s="3" t="s">
         <v>31</v>
       </c>
@@ -2129,17 +2156,17 @@
         <v>109</v>
       </c>
       <c r="J32" s="4"/>
-      <c r="L32" s="39"/>
+      <c r="L32" s="41"/>
       <c r="M32" s="3" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
       <c r="O32" s="4"/>
     </row>
     <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="39"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="3" t="s">
         <v>31</v>
       </c>
@@ -2147,27 +2174,25 @@
         <v>5</v>
       </c>
       <c r="E33" s="4"/>
-      <c r="G33" s="40"/>
+      <c r="G33" s="44"/>
       <c r="H33" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I33" s="3"/>
       <c r="J33" s="4"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N33" s="5"/>
-      <c r="O33" s="6"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="23"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="41"/>
+      <c r="B34" s="42"/>
       <c r="C34" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="6"/>
-      <c r="G34" s="38" t="s">
+      <c r="G34" s="40" t="s">
         <v>66</v>
       </c>
       <c r="H34" s="3" t="s">
@@ -2181,7 +2206,7 @@
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
-      <c r="G35" s="39"/>
+      <c r="G35" s="41"/>
       <c r="H35" s="3" t="s">
         <v>31</v>
       </c>
@@ -2189,7 +2214,7 @@
         <v>110</v>
       </c>
       <c r="J35" s="4"/>
-      <c r="L35" s="42" t="s">
+      <c r="L35" s="43" t="s">
         <v>89</v>
       </c>
       <c r="M35" s="12" t="s">
@@ -2199,7 +2224,7 @@
       <c r="O35" s="13"/>
     </row>
     <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="42" t="s">
+      <c r="B36" s="43" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -2209,23 +2234,23 @@
         <v>6</v>
       </c>
       <c r="E36" s="13"/>
-      <c r="G36" s="41"/>
+      <c r="G36" s="42"/>
       <c r="H36" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I36" s="5"/>
       <c r="J36" s="6"/>
-      <c r="L36" s="39"/>
+      <c r="L36" s="41"/>
       <c r="M36" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O36" s="4"/>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="39"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="3" t="s">
         <v>31</v>
       </c>
@@ -2233,7 +2258,7 @@
         <v>7</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="L37" s="41"/>
+      <c r="L37" s="42"/>
       <c r="M37" s="5" t="s">
         <v>32</v>
       </c>
@@ -2241,7 +2266,7 @@
       <c r="O37" s="6"/>
     </row>
     <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="40"/>
+      <c r="B38" s="44"/>
       <c r="C38" s="3" t="s">
         <v>32</v>
       </c>
@@ -2249,19 +2274,19 @@
         <v>8</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="G38" s="42" t="s">
+      <c r="G38" s="43" t="s">
         <v>67</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J38" s="13"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="40" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2269,23 +2294,25 @@
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
-      <c r="G39" s="39"/>
+      <c r="G39" s="41"/>
       <c r="H39" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="4"/>
-      <c r="L39" s="42" t="s">
+      <c r="L39" s="43" t="s">
         <v>90</v>
       </c>
       <c r="M39" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="N39" s="12"/>
+      <c r="N39" s="12" t="s">
+        <v>177</v>
+      </c>
       <c r="O39" s="13"/>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="39"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="3" t="s">
         <v>31</v>
       </c>
@@ -2293,37 +2320,37 @@
         <v>9</v>
       </c>
       <c r="E40" s="4"/>
-      <c r="G40" s="40"/>
+      <c r="G40" s="44"/>
       <c r="H40" s="34"/>
       <c r="I40" s="34"/>
       <c r="J40" s="22"/>
-      <c r="L40" s="39"/>
+      <c r="L40" s="41"/>
       <c r="M40" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="O40" s="4"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="40"/>
+      <c r="B41" s="44"/>
       <c r="C41" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="4"/>
-      <c r="G41" s="38" t="s">
+      <c r="G41" s="40" t="s">
         <v>68</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="J41" s="4"/>
-      <c r="L41" s="40"/>
+      <c r="L41" s="44"/>
       <c r="M41" s="3" t="s">
         <v>32</v>
       </c>
@@ -2331,7 +2358,7 @@
       <c r="O41" s="4"/>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="40" t="s">
         <v>37</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -2339,13 +2366,13 @@
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
-      <c r="G42" s="39"/>
+      <c r="G42" s="41"/>
       <c r="H42" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" s="4"/>
-      <c r="L42" s="38" t="s">
+      <c r="L42" s="40" t="s">
         <v>91</v>
       </c>
       <c r="M42" s="3" t="s">
@@ -2355,7 +2382,7 @@
       <c r="O42" s="4"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="39"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="3" t="s">
         <v>31</v>
       </c>
@@ -2363,47 +2390,43 @@
         <v>10</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="G43" s="40"/>
+      <c r="G43" s="44"/>
       <c r="H43" s="34"/>
       <c r="I43" s="34"/>
       <c r="J43" s="22"/>
-      <c r="L43" s="39"/>
+      <c r="L43" s="41"/>
       <c r="M43" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N43" s="3" t="s">
-        <v>159</v>
-      </c>
+      <c r="N43" s="3"/>
       <c r="O43" s="4"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="40"/>
+      <c r="B44" s="44"/>
       <c r="C44" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
-      <c r="G44" s="38" t="s">
+      <c r="G44" s="40" t="s">
         <v>69</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J44" s="4"/>
-      <c r="L44" s="40"/>
+      <c r="L44" s="44"/>
       <c r="M44" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N44" s="3" t="s">
-        <v>120</v>
-      </c>
+      <c r="N44" s="57"/>
       <c r="O44" s="4"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="40" t="s">
         <v>38</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2413,23 +2436,25 @@
         <v>11</v>
       </c>
       <c r="E45" s="4"/>
-      <c r="G45" s="39"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I45" s="3"/>
       <c r="J45" s="4"/>
-      <c r="L45" s="38" t="s">
+      <c r="L45" s="40" t="s">
         <v>92</v>
       </c>
       <c r="M45" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N45" s="3"/>
+      <c r="N45" s="3" t="s">
+        <v>179</v>
+      </c>
       <c r="O45" s="4"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="39"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="3" t="s">
         <v>31</v>
       </c>
@@ -2437,21 +2462,21 @@
         <v>11</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="G46" s="40"/>
+      <c r="G46" s="44"/>
       <c r="H46" s="34"/>
       <c r="I46" s="34"/>
       <c r="J46" s="22"/>
-      <c r="L46" s="39"/>
+      <c r="L46" s="41"/>
       <c r="M46" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N46" s="3" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="O46" s="4"/>
     </row>
     <row r="47" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="41"/>
+      <c r="B47" s="42"/>
       <c r="C47" s="5" t="s">
         <v>32</v>
       </c>
@@ -2459,22 +2484,22 @@
         <v>11</v>
       </c>
       <c r="E47" s="6"/>
-      <c r="G47" s="38" t="s">
+      <c r="G47" s="40" t="s">
         <v>70</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="J47" s="4"/>
-      <c r="L47" s="41"/>
+      <c r="L47" s="42"/>
       <c r="M47" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N47" s="5" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
       <c r="O47" s="6"/>
     </row>
@@ -2483,15 +2508,15 @@
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
-      <c r="G48" s="39"/>
+      <c r="G48" s="41"/>
       <c r="H48" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I48" s="3"/>
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="43" t="s">
         <v>39</v>
       </c>
       <c r="C49" s="12" t="s">
@@ -2501,11 +2526,11 @@
         <v>12</v>
       </c>
       <c r="E49" s="13"/>
-      <c r="G49" s="40"/>
+      <c r="G49" s="44"/>
       <c r="H49" s="34"/>
       <c r="I49" s="34"/>
       <c r="J49" s="22"/>
-      <c r="L49" s="42" t="s">
+      <c r="L49" s="43" t="s">
         <v>93</v>
       </c>
       <c r="M49" s="12" t="s">
@@ -2515,7 +2540,7 @@
       <c r="O49" s="13"/>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="39"/>
+      <c r="B50" s="41"/>
       <c r="C50" s="3" t="s">
         <v>31</v>
       </c>
@@ -2523,41 +2548,41 @@
         <v>13</v>
       </c>
       <c r="E50" s="4"/>
-      <c r="G50" s="38" t="s">
+      <c r="G50" s="40" t="s">
         <v>71</v>
       </c>
       <c r="H50" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="I50" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="J50" s="4"/>
-      <c r="L50" s="39"/>
+      <c r="L50" s="41"/>
       <c r="M50" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N50" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="O50" s="4"/>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="40"/>
+      <c r="B51" s="44"/>
       <c r="C51" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="4"/>
-      <c r="G51" s="39"/>
+      <c r="G51" s="41"/>
       <c r="H51" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="J51" s="4"/>
-      <c r="L51" s="40"/>
+      <c r="L51" s="44"/>
       <c r="M51" s="3" t="s">
         <v>32</v>
       </c>
@@ -2565,7 +2590,7 @@
       <c r="O51" s="4"/>
     </row>
     <row r="52" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="38" t="s">
+      <c r="B52" s="40" t="s">
         <v>40</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2573,11 +2598,11 @@
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
-      <c r="G52" s="41"/>
+      <c r="G52" s="42"/>
       <c r="H52" s="35"/>
       <c r="I52" s="35"/>
       <c r="J52" s="23"/>
-      <c r="L52" s="38" t="s">
+      <c r="L52" s="40" t="s">
         <v>94</v>
       </c>
       <c r="M52" s="3" t="s">
@@ -2587,7 +2612,7 @@
       <c r="O52" s="4"/>
     </row>
     <row r="53" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="39"/>
+      <c r="B53" s="41"/>
       <c r="C53" s="3" t="s">
         <v>31</v>
       </c>
@@ -2595,17 +2620,17 @@
         <v>14</v>
       </c>
       <c r="E53" s="4"/>
-      <c r="L53" s="39"/>
+      <c r="L53" s="41"/>
       <c r="M53" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N53" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="O53" s="4"/>
     </row>
     <row r="54" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="40"/>
+      <c r="B54" s="44"/>
       <c r="C54" s="3" t="s">
         <v>32</v>
       </c>
@@ -2613,17 +2638,17 @@
         <v>15</v>
       </c>
       <c r="E54" s="4"/>
-      <c r="G54" s="42" t="s">
+      <c r="G54" s="43" t="s">
         <v>72</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>30</v>
       </c>
       <c r="I54" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J54" s="13"/>
-      <c r="L54" s="41"/>
+      <c r="L54" s="42"/>
       <c r="M54" s="5" t="s">
         <v>32</v>
       </c>
@@ -2631,7 +2656,7 @@
       <c r="O54" s="6"/>
     </row>
     <row r="55" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="38" t="s">
+      <c r="B55" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -2639,17 +2664,17 @@
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="4"/>
-      <c r="G55" s="39"/>
+      <c r="G55" s="41"/>
       <c r="H55" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J55" s="4"/>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="39"/>
+      <c r="B56" s="41"/>
       <c r="C56" s="3" t="s">
         <v>31</v>
       </c>
@@ -2657,15 +2682,15 @@
         <v>16</v>
       </c>
       <c r="E56" s="4"/>
-      <c r="G56" s="40"/>
+      <c r="G56" s="44"/>
       <c r="H56" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J56" s="4"/>
-      <c r="L56" s="42" t="s">
+      <c r="L56" s="43" t="s">
         <v>95</v>
       </c>
       <c r="M56" s="12" t="s">
@@ -2675,7 +2700,7 @@
       <c r="O56" s="13"/>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="40"/>
+      <c r="B57" s="44"/>
       <c r="C57" s="3" t="s">
         <v>32</v>
       </c>
@@ -2688,20 +2713,20 @@
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J57" s="4"/>
-      <c r="L57" s="39"/>
+      <c r="L57" s="41"/>
       <c r="M57" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N57" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O57" s="4"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="38" t="s">
+      <c r="B58" s="40" t="s">
         <v>42</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -2709,7 +2734,7 @@
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="4"/>
-      <c r="G58" s="39" t="s">
+      <c r="G58" s="41" t="s">
         <v>74</v>
       </c>
       <c r="H58" s="7" t="s">
@@ -2717,7 +2742,7 @@
       </c>
       <c r="I58" s="7"/>
       <c r="J58" s="8"/>
-      <c r="L58" s="40"/>
+      <c r="L58" s="44"/>
       <c r="M58" s="3" t="s">
         <v>32</v>
       </c>
@@ -2725,7 +2750,7 @@
       <c r="O58" s="4"/>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="39"/>
+      <c r="B59" s="41"/>
       <c r="C59" s="3" t="s">
         <v>31</v>
       </c>
@@ -2733,7 +2758,7 @@
         <v>18</v>
       </c>
       <c r="E59" s="4"/>
-      <c r="G59" s="39"/>
+      <c r="G59" s="41"/>
       <c r="H59" s="3" t="s">
         <v>31</v>
       </c>
@@ -2741,7 +2766,7 @@
         <v>75</v>
       </c>
       <c r="J59" s="4"/>
-      <c r="L59" s="38" t="s">
+      <c r="L59" s="40" t="s">
         <v>96</v>
       </c>
       <c r="M59" s="3" t="s">
@@ -2751,7 +2776,7 @@
       <c r="O59" s="4"/>
     </row>
     <row r="60" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="41"/>
+      <c r="B60" s="42"/>
       <c r="C60" s="5" t="s">
         <v>32</v>
       </c>
@@ -2759,13 +2784,13 @@
         <v>19</v>
       </c>
       <c r="E60" s="6"/>
-      <c r="G60" s="41"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="6"/>
-      <c r="L60" s="39"/>
+      <c r="L60" s="41"/>
       <c r="M60" s="3" t="s">
         <v>31</v>
       </c>
@@ -2777,7 +2802,7 @@
       <c r="C61" s="15"/>
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
-      <c r="L61" s="40"/>
+      <c r="L61" s="44"/>
       <c r="M61" s="3" t="s">
         <v>32</v>
       </c>
@@ -2785,7 +2810,7 @@
       <c r="O61" s="4"/>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="42" t="s">
+      <c r="B62" s="43" t="s">
         <v>43</v>
       </c>
       <c r="C62" s="12" t="s">
@@ -2793,7 +2818,7 @@
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
-      <c r="G62" s="42" t="s">
+      <c r="G62" s="43" t="s">
         <v>76</v>
       </c>
       <c r="H62" s="12" t="s">
@@ -2801,7 +2826,7 @@
       </c>
       <c r="I62" s="12"/>
       <c r="J62" s="13"/>
-      <c r="L62" s="38" t="s">
+      <c r="L62" s="40" t="s">
         <v>97</v>
       </c>
       <c r="M62" s="3" t="s">
@@ -2811,7 +2836,7 @@
       <c r="O62" s="4"/>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="39"/>
+      <c r="B63" s="41"/>
       <c r="C63" s="3" t="s">
         <v>31</v>
       </c>
@@ -2819,7 +2844,7 @@
         <v>20</v>
       </c>
       <c r="E63" s="4"/>
-      <c r="G63" s="39"/>
+      <c r="G63" s="41"/>
       <c r="H63" s="3" t="s">
         <v>31</v>
       </c>
@@ -2827,29 +2852,29 @@
         <v>111</v>
       </c>
       <c r="J63" s="4"/>
-      <c r="L63" s="39"/>
+      <c r="L63" s="41"/>
       <c r="M63" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N63" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O63" s="4"/>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="40"/>
+      <c r="B64" s="44"/>
       <c r="C64" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
-      <c r="G64" s="40"/>
+      <c r="G64" s="44"/>
       <c r="H64" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="4"/>
-      <c r="L64" s="40"/>
+      <c r="L64" s="44"/>
       <c r="M64" s="3" t="s">
         <v>32</v>
       </c>
@@ -2857,7 +2882,7 @@
       <c r="O64" s="4"/>
     </row>
     <row r="65" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="38" t="s">
+      <c r="B65" s="40" t="s">
         <v>44</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -2865,7 +2890,7 @@
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
-      <c r="G65" s="38" t="s">
+      <c r="G65" s="40" t="s">
         <v>77</v>
       </c>
       <c r="H65" s="3" t="s">
@@ -2878,12 +2903,12 @@
       </c>
       <c r="M65" s="5"/>
       <c r="N65" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O65" s="6"/>
     </row>
     <row r="66" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="39"/>
+      <c r="B66" s="41"/>
       <c r="C66" s="3" t="s">
         <v>31</v>
       </c>
@@ -2891,7 +2916,7 @@
         <v>20</v>
       </c>
       <c r="E66" s="4"/>
-      <c r="G66" s="39"/>
+      <c r="G66" s="41"/>
       <c r="H66" s="3" t="s">
         <v>31</v>
       </c>
@@ -2899,31 +2924,31 @@
       <c r="J66" s="4"/>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="40"/>
+      <c r="B67" s="44"/>
       <c r="C67" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="4"/>
-      <c r="G67" s="40"/>
+      <c r="G67" s="44"/>
       <c r="H67" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I67" s="3"/>
       <c r="J67" s="4"/>
-      <c r="L67" s="42" t="s">
+      <c r="L67" s="43" t="s">
         <v>99</v>
       </c>
       <c r="M67" s="12" t="s">
         <v>30</v>
       </c>
       <c r="N67" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O67" s="13"/>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="38" t="s">
+      <c r="B68" s="40" t="s">
         <v>45</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -2931,7 +2956,7 @@
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="4"/>
-      <c r="G68" s="38" t="s">
+      <c r="G68" s="40" t="s">
         <v>78</v>
       </c>
       <c r="H68" s="3" t="s">
@@ -2939,17 +2964,17 @@
       </c>
       <c r="I68" s="3"/>
       <c r="J68" s="4"/>
-      <c r="L68" s="39"/>
+      <c r="L68" s="41"/>
       <c r="M68" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N68" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O68" s="4"/>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="39"/>
+      <c r="B69" s="41"/>
       <c r="C69" s="3" t="s">
         <v>31</v>
       </c>
@@ -2957,7 +2982,7 @@
         <v>20</v>
       </c>
       <c r="E69" s="4"/>
-      <c r="G69" s="39"/>
+      <c r="G69" s="41"/>
       <c r="H69" s="3" t="s">
         <v>31</v>
       </c>
@@ -2965,29 +2990,29 @@
         <v>112</v>
       </c>
       <c r="J69" s="4"/>
-      <c r="L69" s="40"/>
+      <c r="L69" s="44"/>
       <c r="M69" s="3" t="s">
         <v>32</v>
       </c>
       <c r="N69" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O69" s="4"/>
     </row>
     <row r="70" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="40"/>
+      <c r="B70" s="44"/>
       <c r="C70" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
-      <c r="G70" s="41"/>
+      <c r="G70" s="42"/>
       <c r="H70" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="6"/>
-      <c r="L70" s="38" t="s">
+      <c r="L70" s="40" t="s">
         <v>100</v>
       </c>
       <c r="M70" s="3" t="s">
@@ -2997,7 +3022,7 @@
       <c r="O70" s="4"/>
     </row>
     <row r="71" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="38" t="s">
+      <c r="B71" s="40" t="s">
         <v>46</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -3005,7 +3030,7 @@
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="4"/>
-      <c r="L71" s="39"/>
+      <c r="L71" s="41"/>
       <c r="M71" s="3" t="s">
         <v>31</v>
       </c>
@@ -3013,7 +3038,7 @@
       <c r="O71" s="4"/>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="39"/>
+      <c r="B72" s="41"/>
       <c r="C72" s="3" t="s">
         <v>31</v>
       </c>
@@ -3021,7 +3046,7 @@
         <v>20</v>
       </c>
       <c r="E72" s="4"/>
-      <c r="G72" s="42" t="s">
+      <c r="G72" s="43" t="s">
         <v>79</v>
       </c>
       <c r="H72" s="12" t="s">
@@ -3029,7 +3054,7 @@
       </c>
       <c r="I72" s="12"/>
       <c r="J72" s="13"/>
-      <c r="L72" s="40"/>
+      <c r="L72" s="44"/>
       <c r="M72" s="3" t="s">
         <v>32</v>
       </c>
@@ -3037,13 +3062,13 @@
       <c r="O72" s="4"/>
     </row>
     <row r="73" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="41"/>
+      <c r="B73" s="42"/>
       <c r="C73" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="6"/>
-      <c r="G73" s="39"/>
+      <c r="G73" s="41"/>
       <c r="H73" s="3" t="s">
         <v>31</v>
       </c>
@@ -3051,7 +3076,7 @@
         <v>113</v>
       </c>
       <c r="J73" s="4"/>
-      <c r="L73" s="38" t="s">
+      <c r="L73" s="40" t="s">
         <v>101</v>
       </c>
       <c r="M73" s="3" t="s">
@@ -3065,13 +3090,13 @@
       <c r="C74" s="15"/>
       <c r="D74" s="15"/>
       <c r="E74" s="15"/>
-      <c r="G74" s="40"/>
+      <c r="G74" s="44"/>
       <c r="H74" s="3" t="s">
         <v>32</v>
       </c>
       <c r="I74" s="3"/>
       <c r="J74" s="4"/>
-      <c r="L74" s="39"/>
+      <c r="L74" s="41"/>
       <c r="M74" s="3" t="s">
         <v>31</v>
       </c>
@@ -3079,7 +3104,7 @@
       <c r="O74" s="4"/>
     </row>
     <row r="75" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="43" t="s">
         <v>47</v>
       </c>
       <c r="C75" s="12" t="s">
@@ -3089,7 +3114,7 @@
         <v>21</v>
       </c>
       <c r="E75" s="13"/>
-      <c r="G75" s="38" t="s">
+      <c r="G75" s="40" t="s">
         <v>80</v>
       </c>
       <c r="H75" s="3" t="s">
@@ -3097,7 +3122,7 @@
       </c>
       <c r="I75" s="3"/>
       <c r="J75" s="4"/>
-      <c r="L75" s="41"/>
+      <c r="L75" s="42"/>
       <c r="M75" s="5" t="s">
         <v>32</v>
       </c>
@@ -3105,7 +3130,7 @@
       <c r="O75" s="6"/>
     </row>
     <row r="76" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="39"/>
+      <c r="B76" s="41"/>
       <c r="C76" s="3" t="s">
         <v>31</v>
       </c>
@@ -3113,7 +3138,7 @@
         <v>21</v>
       </c>
       <c r="E76" s="4"/>
-      <c r="G76" s="39"/>
+      <c r="G76" s="41"/>
       <c r="H76" s="3" t="s">
         <v>31</v>
       </c>
@@ -3123,7 +3148,7 @@
       <c r="J76" s="4"/>
     </row>
     <row r="77" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="40"/>
+      <c r="B77" s="44"/>
       <c r="C77" s="3" t="s">
         <v>32</v>
       </c>
@@ -3131,26 +3156,26 @@
         <v>22</v>
       </c>
       <c r="E77" s="31"/>
-      <c r="G77" s="41"/>
+      <c r="G77" s="42"/>
       <c r="H77" s="5" t="s">
         <v>32</v>
       </c>
       <c r="I77" s="5"/>
       <c r="J77" s="6"/>
-      <c r="L77" s="42" t="s">
+      <c r="L77" s="43" t="s">
         <v>102</v>
       </c>
       <c r="M77" s="12" t="s">
         <v>30</v>
       </c>
       <c r="N77" s="12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="O77" s="13"/>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
-      <c r="B78" s="38" t="s">
+      <c r="B78" s="40" t="s">
         <v>48</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -3159,18 +3184,18 @@
       <c r="D78" s="3"/>
       <c r="E78" s="4"/>
       <c r="F78" s="2"/>
-      <c r="L78" s="39"/>
+      <c r="L78" s="41"/>
       <c r="M78" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N78" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="O78" s="4"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
-      <c r="B79" s="39"/>
+      <c r="B79" s="41"/>
       <c r="C79" s="3" t="s">
         <v>31</v>
       </c>
@@ -3179,18 +3204,18 @@
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="2"/>
-      <c r="L79" s="40"/>
+      <c r="L79" s="44"/>
       <c r="M79" s="3" t="s">
         <v>32</v>
       </c>
       <c r="N79" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O79" s="4"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
-      <c r="B80" s="40"/>
+      <c r="B80" s="44"/>
       <c r="C80" s="3" t="s">
         <v>32</v>
       </c>
@@ -3199,7 +3224,7 @@
       </c>
       <c r="E80" s="31"/>
       <c r="F80" s="2"/>
-      <c r="L80" s="38" t="s">
+      <c r="L80" s="40" t="s">
         <v>103</v>
       </c>
       <c r="M80" s="3" t="s">
@@ -3209,7 +3234,7 @@
       <c r="O80" s="4"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B81" s="38" t="s">
+      <c r="B81" s="40" t="s">
         <v>49</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -3217,7 +3242,7 @@
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="4"/>
-      <c r="L81" s="39"/>
+      <c r="L81" s="41"/>
       <c r="M81" s="3" t="s">
         <v>31</v>
       </c>
@@ -3225,15 +3250,15 @@
       <c r="O81" s="4"/>
     </row>
     <row r="82" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="39"/>
+      <c r="B82" s="41"/>
       <c r="C82" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E82" s="4"/>
-      <c r="L82" s="41"/>
+      <c r="L82" s="42"/>
       <c r="M82" s="5" t="s">
         <v>32</v>
       </c>
@@ -3241,7 +3266,7 @@
       <c r="O82" s="6"/>
     </row>
     <row r="83" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="40"/>
+      <c r="B83" s="44"/>
       <c r="C83" s="3" t="s">
         <v>32</v>
       </c>
@@ -3251,8 +3276,8 @@
       <c r="E83" s="31"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B84" s="38" t="s">
-        <v>142</v>
+      <c r="B84" s="40" t="s">
+        <v>139</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>30</v>
@@ -3261,37 +3286,37 @@
         <v>0</v>
       </c>
       <c r="E84" s="4"/>
-      <c r="L84" s="42" t="s">
+      <c r="L84" s="43" t="s">
         <v>104</v>
       </c>
       <c r="M84" s="12" t="s">
         <v>30</v>
       </c>
       <c r="N84" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O84" s="13"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="39"/>
+      <c r="B85" s="41"/>
       <c r="C85" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E85" s="4"/>
-      <c r="L85" s="39"/>
+      <c r="L85" s="41"/>
       <c r="M85" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N85" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="O85" s="4"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B86" s="40"/>
+      <c r="B86" s="44"/>
       <c r="C86" s="3" t="s">
         <v>32</v>
       </c>
@@ -3299,7 +3324,7 @@
         <v>0</v>
       </c>
       <c r="E86" s="4"/>
-      <c r="L86" s="40"/>
+      <c r="L86" s="44"/>
       <c r="M86" s="3" t="s">
         <v>32</v>
       </c>
@@ -3307,7 +3332,7 @@
       <c r="O86" s="4"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B87" s="38" t="s">
+      <c r="B87" s="40" t="s">
         <v>50</v>
       </c>
       <c r="C87" s="3" t="s">
@@ -3315,8 +3340,8 @@
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="4"/>
-      <c r="L87" s="38" t="s">
-        <v>129</v>
+      <c r="L87" s="40" t="s">
+        <v>126</v>
       </c>
       <c r="M87" s="3" t="s">
         <v>30</v>
@@ -3325,7 +3350,7 @@
       <c r="O87" s="4"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88" s="39"/>
+      <c r="B88" s="41"/>
       <c r="C88" s="3" t="s">
         <v>31</v>
       </c>
@@ -3333,7 +3358,7 @@
         <v>26</v>
       </c>
       <c r="E88" s="4"/>
-      <c r="L88" s="39"/>
+      <c r="L88" s="41"/>
       <c r="M88" s="3" t="s">
         <v>31</v>
       </c>
@@ -3341,7 +3366,7 @@
       <c r="O88" s="4"/>
     </row>
     <row r="89" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="40"/>
+      <c r="B89" s="44"/>
       <c r="C89" s="3" t="s">
         <v>32</v>
       </c>
@@ -3349,7 +3374,7 @@
         <v>27</v>
       </c>
       <c r="E89" s="31"/>
-      <c r="L89" s="41"/>
+      <c r="L89" s="42"/>
       <c r="M89" s="5" t="s">
         <v>32</v>
       </c>
@@ -3357,27 +3382,27 @@
       <c r="O89" s="6"/>
     </row>
     <row r="90" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="38" t="s">
+      <c r="B90" s="40" t="s">
         <v>28</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E90" s="4"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B91" s="39"/>
+      <c r="B91" s="41"/>
       <c r="C91" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E91" s="4"/>
-      <c r="L91" s="42" t="s">
+      <c r="L91" s="43" t="s">
         <v>105</v>
       </c>
       <c r="M91" s="12" t="s">
@@ -3387,25 +3412,25 @@
       <c r="O91" s="13"/>
     </row>
     <row r="92" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="41"/>
+      <c r="B92" s="42"/>
       <c r="C92" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E92" s="6"/>
-      <c r="L92" s="39"/>
+      <c r="L92" s="41"/>
       <c r="M92" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N92" s="3"/>
       <c r="O92" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L93" s="40"/>
+      <c r="L93" s="44"/>
       <c r="M93" s="3" t="s">
         <v>32</v>
       </c>
@@ -3413,7 +3438,7 @@
       <c r="O93" s="4"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L94" s="38" t="s">
+      <c r="L94" s="40" t="s">
         <v>106</v>
       </c>
       <c r="M94" s="3" t="s">
@@ -3423,17 +3448,17 @@
       <c r="O94" s="4"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L95" s="39"/>
+      <c r="L95" s="41"/>
       <c r="M95" s="3" t="s">
         <v>31</v>
       </c>
       <c r="N95" s="3"/>
       <c r="O95" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="96" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L96" s="41"/>
+      <c r="L96" s="42"/>
       <c r="M96" s="5" t="s">
         <v>32</v>
       </c>
@@ -3442,7 +3467,7 @@
     </row>
     <row r="97" spans="12:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L98" s="42" t="s">
+      <c r="L98" s="43" t="s">
         <v>107</v>
       </c>
       <c r="M98" s="12" t="s">
@@ -3452,7 +3477,7 @@
       <c r="O98" s="13"/>
     </row>
     <row r="99" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L99" s="39"/>
+      <c r="L99" s="41"/>
       <c r="M99" s="3" t="s">
         <v>31</v>
       </c>
@@ -3460,7 +3485,7 @@
       <c r="O99" s="4"/>
     </row>
     <row r="100" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L100" s="40"/>
+      <c r="L100" s="44"/>
       <c r="M100" s="3" t="s">
         <v>32</v>
       </c>
@@ -3468,7 +3493,7 @@
       <c r="O100" s="4"/>
     </row>
     <row r="101" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L101" s="38" t="s">
+      <c r="L101" s="40" t="s">
         <v>108</v>
       </c>
       <c r="M101" s="3" t="s">
@@ -3478,7 +3503,7 @@
       <c r="O101" s="4"/>
     </row>
     <row r="102" spans="12:15" x14ac:dyDescent="0.25">
-      <c r="L102" s="39"/>
+      <c r="L102" s="41"/>
       <c r="M102" s="3" t="s">
         <v>31</v>
       </c>
@@ -3486,7 +3511,7 @@
       <c r="O102" s="4"/>
     </row>
     <row r="103" spans="12:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L103" s="41"/>
+      <c r="L103" s="42"/>
       <c r="M103" s="5" t="s">
         <v>32</v>
       </c>
@@ -3495,36 +3520,35 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="L87:L89"/>
-    <mergeCell ref="L91:L93"/>
-    <mergeCell ref="L94:L96"/>
-    <mergeCell ref="L98:L100"/>
-    <mergeCell ref="L101:L103"/>
-    <mergeCell ref="B2:O2"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="B7:B12"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="G58:G60"/>
-    <mergeCell ref="G62:G64"/>
+    <mergeCell ref="L80:L82"/>
+    <mergeCell ref="G72:G74"/>
+    <mergeCell ref="G75:G77"/>
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="L24:L26"/>
+    <mergeCell ref="L27:L29"/>
+    <mergeCell ref="L31:L33"/>
+    <mergeCell ref="L49:L51"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="L39:L41"/>
+    <mergeCell ref="L42:L44"/>
+    <mergeCell ref="B87:B89"/>
+    <mergeCell ref="L84:L86"/>
+    <mergeCell ref="L67:L69"/>
+    <mergeCell ref="L52:L54"/>
+    <mergeCell ref="L56:L58"/>
+    <mergeCell ref="L59:L61"/>
+    <mergeCell ref="L62:L64"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="G68:G70"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="L70:L72"/>
+    <mergeCell ref="L73:L75"/>
+    <mergeCell ref="L77:L79"/>
+    <mergeCell ref="L45:L47"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="G47:G49"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="G54:G56"/>
     <mergeCell ref="B90:B92"/>
     <mergeCell ref="G21:G23"/>
     <mergeCell ref="G25:G27"/>
@@ -3539,39 +3563,40 @@
     <mergeCell ref="B75:B77"/>
     <mergeCell ref="B78:B80"/>
     <mergeCell ref="B81:B83"/>
-    <mergeCell ref="L45:L47"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="G47:G49"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="G58:G60"/>
+    <mergeCell ref="G62:G64"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="G4:J4"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="L10:L12"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="L39:L41"/>
-    <mergeCell ref="L42:L44"/>
-    <mergeCell ref="B87:B89"/>
-    <mergeCell ref="L84:L86"/>
-    <mergeCell ref="L67:L69"/>
     <mergeCell ref="L13:L15"/>
     <mergeCell ref="L17:L19"/>
-    <mergeCell ref="L20:L22"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="L27:L29"/>
-    <mergeCell ref="L31:L33"/>
-    <mergeCell ref="L49:L51"/>
-    <mergeCell ref="L52:L54"/>
-    <mergeCell ref="L56:L58"/>
-    <mergeCell ref="L59:L61"/>
-    <mergeCell ref="L62:L64"/>
-    <mergeCell ref="G65:G67"/>
-    <mergeCell ref="G68:G70"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="L70:L72"/>
-    <mergeCell ref="L73:L75"/>
-    <mergeCell ref="L77:L79"/>
-    <mergeCell ref="L80:L82"/>
-    <mergeCell ref="G72:G74"/>
-    <mergeCell ref="G75:G77"/>
+    <mergeCell ref="L87:L89"/>
+    <mergeCell ref="L91:L93"/>
+    <mergeCell ref="L94:L96"/>
+    <mergeCell ref="L98:L100"/>
+    <mergeCell ref="L101:L103"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>